<commit_message>
#added hand sieved data to the analyzer data
</commit_message>
<xml_diff>
--- a/hand_sieved_data.xlsx
+++ b/hand_sieved_data.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ardowney\Documents\PROTECT sediment\data\PARTICLE ANALYSIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/autumdowney/Desktop/ESDA/exercises/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="10725"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="18940" windowHeight="10720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -390,9 +396,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -425,9 +431,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -609,38 +615,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
       <selection activeCell="Q171" sqref="Q171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -665,7 +671,7 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -712,7 +718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -762,7 +768,7 @@
         <v>1.1713</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -812,7 +818,7 @@
         <v>0.93530000000000024</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -862,7 +868,7 @@
         <v>1.0355000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>25</v>
       </c>
@@ -903,7 +909,7 @@
         <v>0.61830000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>26</v>
       </c>
@@ -944,7 +950,7 @@
         <v>1.2065999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>27</v>
       </c>
@@ -985,7 +991,7 @@
         <v>5.1798000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>28</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>78.349999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="H12">
         <f>SUM(H5:H11)</f>
         <v>92.146300000000039</v>
@@ -1041,7 +1047,7 @@
         <v>88.496799999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>31</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>10.292143943233667</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1096,7 @@
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
     </row>
-    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>2.1500000000000075E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1225,7 +1231,7 @@
         <v>2.3299999999999876E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1269,7 +1275,7 @@
         <v>4.0899999999999714E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>8.9800000000000324E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>26</v>
       </c>
@@ -1339,7 +1345,7 @@
         <v>0.60840000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>27</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>6.4549000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>28</v>
       </c>
@@ -1409,7 +1415,7 @@
         <v>85.7</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="H24">
         <f>SUM(H17:H23)</f>
         <v>0</v>
@@ -1423,7 +1429,7 @@
         <v>92.938800000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>7.8262421898244545</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>32</v>
       </c>
@@ -1470,7 +1476,7 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>2.5695000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>9.8474000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1667,7 +1673,7 @@
         <v>34.996000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>42</v>
       </c>
@@ -1708,7 +1714,7 @@
         <v>18.883499999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
         <v>43</v>
       </c>
@@ -1749,7 +1755,7 @@
         <v>3.9396000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E34" t="s">
         <v>44</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>1.2780999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
         <v>45</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>-1.1099999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F36">
         <v>15.33</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>-1.3999999999999986</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F37">
         <v>15.46</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>-1.3500000000000014</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F38">
         <v>15.23</v>
       </c>
@@ -1927,7 +1933,7 @@
         <v>-0.36000000000000298</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F39">
         <v>15.25</v>
       </c>
@@ -1959,7 +1965,7 @@
         <v>-0.83999999999999986</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
         <v>46</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>-1.2000000000000011</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
         <v>31</v>
       </c>
@@ -2015,7 +2021,7 @@
         <v>-0.66000000000000014</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P42">
         <v>17.21</v>
       </c>
@@ -2027,7 +2033,7 @@
         <v>3.7399999999999984</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P43">
         <v>17.059999999999999</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>-0.41999999999999815</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P44">
         <v>17.23</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>13.969999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O45" t="s">
         <v>46</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>81.884099999999989</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O46" t="s">
         <v>31</v>
       </c>
@@ -2070,7 +2076,7 @@
       </c>
       <c r="Q46" s="10"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>10</v>
       </c>
@@ -2094,7 +2100,7 @@
       <c r="P48" s="10"/>
       <c r="Q48" s="10"/>
     </row>
-    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>0.27360000000000007</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2241,7 +2247,7 @@
         <v>0.29479999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -2291,7 +2297,7 @@
         <v>3.3401000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E53" t="s">
         <v>42</v>
       </c>
@@ -2332,7 +2338,7 @@
         <v>8.5509999999999984</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
         <v>43</v>
       </c>
@@ -2373,7 +2379,7 @@
         <v>12.571300000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E55" t="s">
         <v>44</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>2.7968999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
         <v>45</v>
       </c>
@@ -2455,7 +2461,7 @@
         <v>4.1099999999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F57">
         <v>15.8</v>
       </c>
@@ -2487,7 +2493,7 @@
         <v>7.8900000000000006</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F58">
         <v>15.81</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>4.6499999999999986</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F59">
         <v>16.79</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
         <v>46</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>48.797699999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
         <v>31</v>
       </c>
@@ -2592,7 +2598,7 @@
       </c>
       <c r="Q61" s="10"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>14</v>
       </c>
@@ -2616,7 +2622,7 @@
       <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
     </row>
-    <row r="64" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>1</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -2713,7 +2719,7 @@
         <v>0.14339999999999975</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2763,7 +2769,7 @@
         <v>6.7499999999999893E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -2813,7 +2819,7 @@
         <v>0.28349999999999964</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
         <v>42</v>
       </c>
@@ -2854,7 +2860,7 @@
         <v>1.1383000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E69" t="s">
         <v>43</v>
       </c>
@@ -2895,7 +2901,7 @@
         <v>3.8053999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E70" t="s">
         <v>44</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>7.4832999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E71" t="s">
         <v>45</v>
       </c>
@@ -2977,7 +2983,7 @@
         <v>0.75999999999999979</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F72">
         <v>15.93</v>
       </c>
@@ -3009,7 +3015,7 @@
         <v>4.8699999999999992</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F73">
         <v>16.13</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>31.730000000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F74">
         <v>16.25</v>
       </c>
@@ -3070,7 +3076,7 @@
         <v>50.281400000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E75" t="s">
         <v>46</v>
       </c>
@@ -3094,7 +3100,7 @@
       </c>
       <c r="Q75" s="10"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E76" t="s">
         <v>31</v>
       </c>
@@ -3114,7 +3120,7 @@
       <c r="L76" s="10"/>
       <c r="M76" s="4"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>48</v>
       </c>
@@ -3138,7 +3144,7 @@
       <c r="P78" s="10"/>
       <c r="Q78" s="10"/>
     </row>
-    <row r="79" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>1</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -3235,7 +3241,7 @@
         <v>0.11539999999999973</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -3285,7 +3291,7 @@
         <v>0.45500000000000007</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -3334,7 +3340,7 @@
         <v>3.9331</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E83" s="7" t="s">
         <v>42</v>
       </c>
@@ -3375,7 +3381,7 @@
         <v>12.8538</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E84" s="7" t="s">
         <v>43</v>
       </c>
@@ -3416,7 +3422,7 @@
         <v>17.895599999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E85" s="7" t="s">
         <v>44</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>13.052299999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E86" s="7" t="s">
         <v>45</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>5.7299999999999986</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E87" s="7"/>
       <c r="F87" s="7">
         <v>342.15</v>
@@ -3531,7 +3537,7 @@
         <v>12.420000000000002</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E88" s="7" t="s">
         <v>46</v>
       </c>
@@ -3562,7 +3568,7 @@
         <v>10.87</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E89" s="7" t="s">
         <v>31</v>
       </c>
@@ -3593,7 +3599,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K90">
         <v>12</v>
       </c>
@@ -3615,7 +3621,7 @@
         <v>8.9799999999999986</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E91" s="12" t="s">
         <v>53</v>
       </c>
@@ -3644,7 +3650,7 @@
         <v>7.4599999999999991</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J92" t="s">
         <v>46</v>
       </c>
@@ -3660,7 +3666,7 @@
         <v>102.40519999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J93" t="s">
         <v>31</v>
       </c>
@@ -3679,7 +3685,7 @@
       </c>
       <c r="Q93" s="5"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
         <v>54</v>
       </c>
@@ -3703,7 +3709,7 @@
       <c r="P95" s="10"/>
       <c r="Q95" s="10"/>
     </row>
-    <row r="96" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>1</v>
       </c>
@@ -3750,7 +3756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -3800,7 +3806,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>56</v>
       </c>
@@ -3850,7 +3856,7 @@
         <v>9.4780999999999995</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>57</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>25.441500000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
         <v>42</v>
       </c>
@@ -3941,7 +3947,7 @@
         <v>9.4461999999999993</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E101" t="s">
         <v>43</v>
       </c>
@@ -3982,7 +3988,7 @@
         <v>0.35009999999999986</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E102" t="s">
         <v>44</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E103" t="s">
         <v>45</v>
       </c>
@@ -4064,7 +4070,7 @@
         <v>3.7899999999999991</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F104">
         <v>12.28</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>4.5199999999999978</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O106" t="s">
         <v>46</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>54.033899999999988</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E107" t="s">
         <v>46</v>
       </c>
@@ -4129,7 +4135,7 @@
       </c>
       <c r="Q107" s="10"/>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E108" t="s">
         <v>31</v>
       </c>
@@ -4149,7 +4155,7 @@
       <c r="L108" s="10"/>
       <c r="M108" s="9"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
         <v>58</v>
       </c>
@@ -4173,7 +4179,7 @@
       <c r="P110" s="10"/>
       <c r="Q110" s="10"/>
     </row>
-    <row r="111" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>1</v>
       </c>
@@ -4220,7 +4226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>59</v>
       </c>
@@ -4270,7 +4276,7 @@
         <v>0.49699999999999989</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>60</v>
       </c>
@@ -4320,7 +4326,7 @@
         <v>0.4403999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>61</v>
       </c>
@@ -4370,7 +4376,7 @@
         <v>0.49570000000000025</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E115" t="s">
         <v>42</v>
       </c>
@@ -4411,7 +4417,7 @@
         <v>0.51089999999999991</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E116" t="s">
         <v>43</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>0.78120000000000012</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E117" t="s">
         <v>44</v>
       </c>
@@ -4493,7 +4499,7 @@
         <v>2.5842999999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E118" t="s">
         <v>45</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>29.96</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F119">
         <v>12.1</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>8.8399999999999981</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F120">
         <v>12.08</v>
       </c>
@@ -4598,7 +4604,7 @@
         <v>5.6399999999999988</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O121" t="s">
         <v>46</v>
       </c>
@@ -4607,7 +4613,7 @@
         <v>49.749499999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E122" t="s">
         <v>46</v>
       </c>
@@ -4631,7 +4637,7 @@
       </c>
       <c r="Q122" s="10"/>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E123" t="s">
         <v>31</v>
       </c>
@@ -4651,7 +4657,7 @@
       <c r="L123" s="10"/>
       <c r="M123" s="9"/>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
         <v>62</v>
       </c>
@@ -4675,7 +4681,7 @@
       <c r="P126" s="10"/>
       <c r="Q126" s="10"/>
     </row>
-    <row r="127" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
@@ -4722,7 +4728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>64</v>
       </c>
@@ -4772,7 +4778,7 @@
         <v>1.1730999999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>63</v>
       </c>
@@ -4822,7 +4828,7 @@
         <v>0.17749999999999977</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>65</v>
       </c>
@@ -4872,7 +4878,7 @@
         <v>0.13400000000000034</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E131" t="s">
         <v>42</v>
       </c>
@@ -4913,7 +4919,7 @@
         <v>0.29739999999999966</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E132" t="s">
         <v>43</v>
       </c>
@@ -4954,7 +4960,7 @@
         <v>1.4421999999999997</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E133" t="s">
         <v>44</v>
       </c>
@@ -4995,7 +5001,7 @@
         <v>13.7455</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E134" t="s">
         <v>45</v>
       </c>
@@ -5036,7 +5042,7 @@
         <v>4.2600000000000016</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F135">
         <v>12.04</v>
       </c>
@@ -5068,7 +5074,7 @@
         <v>28.44</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O137" t="s">
         <v>46</v>
       </c>
@@ -5077,7 +5083,7 @@
         <v>49.669700000000006</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E138" t="s">
         <v>46</v>
       </c>
@@ -5101,7 +5107,7 @@
       </c>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E139" t="s">
         <v>31</v>
       </c>
@@ -5121,7 +5127,7 @@
       <c r="L139" s="10"/>
       <c r="M139" s="9"/>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" s="10" t="s">
         <v>68</v>
       </c>
@@ -5145,7 +5151,7 @@
       <c r="P142" s="10"/>
       <c r="Q142" s="10"/>
     </row>
-    <row r="143" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>1</v>
       </c>
@@ -5192,7 +5198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>69</v>
       </c>
@@ -5242,7 +5248,7 @@
         <v>3.8477999999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>70</v>
       </c>
@@ -5292,7 +5298,7 @@
         <v>0.1177999999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>71</v>
       </c>
@@ -5342,7 +5348,7 @@
         <v>0.11430000000000007</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E147" t="s">
         <v>42</v>
       </c>
@@ -5383,7 +5389,7 @@
         <v>0.12709999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E148" t="s">
         <v>43</v>
       </c>
@@ -5424,7 +5430,7 @@
         <v>3.8607999999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E149" t="s">
         <v>44</v>
       </c>
@@ -5465,7 +5471,7 @@
         <v>15.739700000000003</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E150" t="s">
         <v>45</v>
       </c>
@@ -5496,7 +5502,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F151">
         <v>12.14</v>
       </c>
@@ -5528,7 +5534,7 @@
         <v>20.759999999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P152">
         <v>12.28</v>
       </c>
@@ -5540,7 +5546,7 @@
         <v>5.4599999999999991</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O153" t="s">
         <v>46</v>
       </c>
@@ -5549,7 +5555,7 @@
         <v>50.027500000000003</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E154" t="s">
         <v>46</v>
       </c>
@@ -5573,7 +5579,7 @@
       </c>
       <c r="Q154" s="10"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E155" t="s">
         <v>31</v>
       </c>
@@ -5593,7 +5599,7 @@
       <c r="L155" s="10"/>
       <c r="M155" s="9"/>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" s="10" t="s">
         <v>72</v>
       </c>
@@ -5617,7 +5623,7 @@
       <c r="P158" s="10"/>
       <c r="Q158" s="10"/>
     </row>
-    <row r="159" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" ht="30" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>1</v>
       </c>
@@ -5664,7 +5670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>73</v>
       </c>
@@ -5714,7 +5720,7 @@
         <v>3.9400000000000102E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>74</v>
       </c>
@@ -5764,7 +5770,7 @@
         <v>7.4400000000000244E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>75</v>
       </c>
@@ -5814,7 +5820,7 @@
         <v>0.14290000000000003</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E163" t="s">
         <v>42</v>
       </c>
@@ -5855,7 +5861,7 @@
         <v>8.3000000000000185E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E164" t="s">
         <v>43</v>
       </c>
@@ -5896,7 +5902,7 @@
         <v>0.2168000000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E165" t="s">
         <v>44</v>
       </c>
@@ -5937,7 +5943,7 @@
         <v>0.38890000000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E166" t="s">
         <v>45</v>
       </c>
@@ -5978,7 +5984,7 @@
         <v>4.8499999999999979</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F167">
         <v>12.17</v>
       </c>
@@ -6010,7 +6016,7 @@
         <v>5.9599999999999991</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F168">
         <v>12.08</v>
       </c>
@@ -6042,7 +6048,7 @@
         <v>4.3599999999999994</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F169">
         <v>12.16</v>
       </c>
@@ -6074,7 +6080,7 @@
         <v>7.3299999999999983</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E170" t="s">
         <v>46</v>
       </c>
@@ -6100,7 +6106,7 @@
         <v>26.490000000000009</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E171" t="s">
         <v>31</v>
       </c>
@@ -6127,7 +6133,7 @@
         <v>49.935400000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O172" t="s">
         <v>31</v>
       </c>
@@ -6139,27 +6145,40 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="J78:L78"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="J63:L63"/>
-    <mergeCell ref="O78:Q78"/>
-    <mergeCell ref="P75:Q75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="K93:L93"/>
-    <mergeCell ref="E91:H91"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="O48:Q48"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="O63:Q63"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="F171:G171"/>
+    <mergeCell ref="K171:L171"/>
+    <mergeCell ref="P154:Q154"/>
+    <mergeCell ref="F155:G155"/>
+    <mergeCell ref="K155:L155"/>
+    <mergeCell ref="A158:C158"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="J158:L158"/>
+    <mergeCell ref="O158:Q158"/>
+    <mergeCell ref="P138:Q138"/>
+    <mergeCell ref="F139:G139"/>
+    <mergeCell ref="K139:L139"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="E142:G142"/>
+    <mergeCell ref="J142:L142"/>
+    <mergeCell ref="O142:Q142"/>
+    <mergeCell ref="O110:Q110"/>
+    <mergeCell ref="P122:Q122"/>
+    <mergeCell ref="F123:G123"/>
+    <mergeCell ref="K123:L123"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="E126:G126"/>
+    <mergeCell ref="J126:L126"/>
+    <mergeCell ref="O126:Q126"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="K108:L108"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="E110:G110"/>
+    <mergeCell ref="J110:L110"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="J95:L95"/>
+    <mergeCell ref="O95:Q95"/>
+    <mergeCell ref="P107:Q107"/>
     <mergeCell ref="A48:C48"/>
     <mergeCell ref="P46:Q46"/>
     <mergeCell ref="A1:C1"/>
@@ -6176,40 +6195,27 @@
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="J15:M15"/>
-    <mergeCell ref="A95:C95"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="J95:L95"/>
-    <mergeCell ref="O95:Q95"/>
-    <mergeCell ref="P107:Q107"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="K108:L108"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="E110:G110"/>
-    <mergeCell ref="J110:L110"/>
-    <mergeCell ref="O110:Q110"/>
-    <mergeCell ref="P122:Q122"/>
-    <mergeCell ref="F123:G123"/>
-    <mergeCell ref="K123:L123"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="E126:G126"/>
-    <mergeCell ref="J126:L126"/>
-    <mergeCell ref="O126:Q126"/>
-    <mergeCell ref="A158:C158"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="J158:L158"/>
-    <mergeCell ref="O158:Q158"/>
-    <mergeCell ref="P138:Q138"/>
-    <mergeCell ref="F139:G139"/>
-    <mergeCell ref="K139:L139"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="E142:G142"/>
-    <mergeCell ref="J142:L142"/>
-    <mergeCell ref="O142:Q142"/>
-    <mergeCell ref="F171:G171"/>
-    <mergeCell ref="K171:L171"/>
-    <mergeCell ref="P154:Q154"/>
-    <mergeCell ref="F155:G155"/>
-    <mergeCell ref="K155:L155"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="O48:Q48"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="O63:Q63"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="O78:Q78"/>
+    <mergeCell ref="P75:Q75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="K93:L93"/>
+    <mergeCell ref="E91:H91"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="J78:L78"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="J63:L63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>